<commit_message>
Updating with measurement noise
</commit_message>
<xml_diff>
--- a/tiv_model/SimulatedViralLoad.xlsx
+++ b/tiv_model/SimulatedViralLoad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttcas\Dropbox\MATLAB\Identifiability of population models\HIV Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5877114-2099-4633-91C4-3FA082EAD885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354B773C-075A-4EB5-8D39-FCE7DF289B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{48EC7B78-4689-47A1-9278-BEAAA98E39DC}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Viral load</t>
+    <t>log10 Viral load</t>
   </si>
 </sst>
 </file>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A5F873-D764-4840-90FC-6826FE23133F}">
   <dimension ref="A1:C270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
-      <selection activeCell="E262" sqref="E262"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="A271" sqref="A271:XFD271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.2714330829818301</v>
+        <v>1.3224273763465599</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>7.38034160488324</v>
+        <v>7.1719190684147502</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -465,7 +465,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>6.8233609904144297</v>
+        <v>6.7856864007065596</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -476,7 +476,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>6.3392009404381504</v>
+        <v>6.4072466144097797</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -487,7 +487,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>6.0083928240267497</v>
+        <v>6.0416965390435697</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>5.8610093736490798</v>
+        <v>5.9684094695898198</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -509,7 +509,7 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>5.8243476426887497</v>
+        <v>6.1769112458550302</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -520,7 +520,7 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>5.8197302392681598</v>
+        <v>5.8443743352531499</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -531,7 +531,7 @@
         <v>32</v>
       </c>
       <c r="C10">
-        <v>5.8195248254135503</v>
+        <v>5.8100239483904197</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -542,7 +542,7 @@
         <v>36</v>
       </c>
       <c r="C11">
-        <v>5.8195491170801104</v>
+        <v>5.8297059610322304</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -553,7 +553,7 @@
         <v>40</v>
       </c>
       <c r="C12">
-        <v>5.8195540838163096</v>
+        <v>5.8476415886894602</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -564,7 +564,7 @@
         <v>44</v>
       </c>
       <c r="C13">
-        <v>5.81955440306381</v>
+        <v>5.8588155355483202</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -575,7 +575,7 @@
         <v>48</v>
       </c>
       <c r="C14">
-        <v>5.8195543878186502</v>
+        <v>5.9127853488500701</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -586,7 +586,7 @@
         <v>52</v>
       </c>
       <c r="C15">
-        <v>5.8195543827022602</v>
+        <v>5.7847350633880898</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -597,7 +597,7 @@
         <v>56</v>
       </c>
       <c r="C16">
-        <v>5.8195543822706401</v>
+        <v>5.7756434048890997</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -608,7 +608,7 @@
         <v>60</v>
       </c>
       <c r="C17">
-        <v>5.8195543822744602</v>
+        <v>5.92311256705944</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -619,7 +619,7 @@
         <v>64</v>
       </c>
       <c r="C18">
-        <v>5.8195543822794402</v>
+        <v>5.64497251113837</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.76520235877641096</v>
+        <v>0.81930369376927603</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -641,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <v>7.7885411331172598</v>
+        <v>7.9085070472541696</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -652,7 +652,7 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>7.2680308896180303</v>
+        <v>7.2965043452289402</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="C23">
-        <v>6.8650093053399601</v>
+        <v>6.9076700789143501</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -674,7 +674,7 @@
         <v>16</v>
       </c>
       <c r="C24">
-        <v>6.6437674722344298</v>
+        <v>6.4529856807237502</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -685,7 +685,7 @@
         <v>20</v>
       </c>
       <c r="C25">
-        <v>6.5720860676591197</v>
+        <v>6.5628236974829397</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -696,7 +696,7 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>6.56042480970157</v>
+        <v>6.7149083237506799</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -707,7 +707,7 @@
         <v>28</v>
       </c>
       <c r="C27">
-        <v>6.5598053296344698</v>
+        <v>6.40994280393297</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>6.5598948581414902</v>
+        <v>6.67772816744887</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -729,7 +729,7 @@
         <v>36</v>
       </c>
       <c r="C29">
-        <v>6.5599135836101903</v>
+        <v>6.6437885362555296</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -740,7 +740,7 @@
         <v>40</v>
       </c>
       <c r="C30">
-        <v>6.5599144391994102</v>
+        <v>6.8027109235219001</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -751,7 +751,7 @@
         <v>44</v>
       </c>
       <c r="C31">
-        <v>6.5599142738554397</v>
+        <v>6.5747355919042096</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -762,7 +762,7 @@
         <v>48</v>
       </c>
       <c r="C32">
-        <v>6.5599142432975004</v>
+        <v>6.5098943020812596</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -773,7 +773,7 @@
         <v>52</v>
       </c>
       <c r="C33">
-        <v>6.5599142421690404</v>
+        <v>6.6067620839049397</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -784,7 +784,7 @@
         <v>56</v>
       </c>
       <c r="C34">
-        <v>6.5599142424689703</v>
+        <v>6.4322127337519204</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -795,7 +795,7 @@
         <v>60</v>
       </c>
       <c r="C35">
-        <v>6.5599142425184898</v>
+        <v>6.7177771961492798</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -806,7 +806,7 @@
         <v>64</v>
       </c>
       <c r="C36">
-        <v>6.55991424251987</v>
+        <v>6.5853506913288804</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>0.76396795174944498</v>
+        <v>0.92828110501683003</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -828,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="C39">
-        <v>8.3480795141648798</v>
+        <v>8.3578741935552401</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -839,7 +839,7 @@
         <v>8</v>
       </c>
       <c r="C40">
-        <v>7.7936044662719803</v>
+        <v>7.8266575378669998</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -850,7 +850,7 @@
         <v>12</v>
       </c>
       <c r="C41">
-        <v>7.3459202147561804</v>
+        <v>7.3336819036801497</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -861,7 +861,7 @@
         <v>16</v>
       </c>
       <c r="C42">
-        <v>7.0871890945046498</v>
+        <v>7.1442121580872504</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -872,7 +872,7 @@
         <v>20</v>
       </c>
       <c r="C43">
-        <v>6.9892625180893502</v>
+        <v>6.7732749343255296</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -883,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="C44">
-        <v>6.9613738930992204</v>
+        <v>7.0237122201900997</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -894,7 +894,7 @@
         <v>28</v>
       </c>
       <c r="C45">
-        <v>6.9542674631590504</v>
+        <v>6.91236900718767</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -905,7 +905,7 @@
         <v>32</v>
       </c>
       <c r="C46">
-        <v>6.9525134380716702</v>
+        <v>7.0123917992529803</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -916,7 +916,7 @@
         <v>36</v>
       </c>
       <c r="C47">
-        <v>6.9520840113261304</v>
+        <v>7.0536831749439504</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -927,7 +927,7 @@
         <v>40</v>
       </c>
       <c r="C48">
-        <v>6.95197908844521</v>
+        <v>6.7719621590555503</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -938,7 +938,7 @@
         <v>44</v>
       </c>
       <c r="C49">
-        <v>6.9519534650104404</v>
+        <v>6.9678251443491801</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -949,7 +949,7 @@
         <v>48</v>
       </c>
       <c r="C50">
-        <v>6.9519472082096296</v>
+        <v>7.0202083527771499</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -960,7 +960,7 @@
         <v>52</v>
       </c>
       <c r="C51">
-        <v>6.9519456804515896</v>
+        <v>7.0014780239338501</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -971,7 +971,7 @@
         <v>56</v>
       </c>
       <c r="C52">
-        <v>6.9519453074130402</v>
+        <v>7.1678265178746203</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -982,7 +982,7 @@
         <v>60</v>
       </c>
       <c r="C53">
-        <v>6.9519452163269504</v>
+        <v>6.9882489781739903</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -993,7 +993,7 @@
         <v>64</v>
       </c>
       <c r="C54">
-        <v>6.9519451940861501</v>
+        <v>6.8176147235189797</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>1.3655336434865599</v>
+        <v>1.2776007201047499</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="C57">
-        <v>8.9577024683763309</v>
+        <v>8.8527156288708699</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -1026,7 +1026,7 @@
         <v>8</v>
       </c>
       <c r="C58">
-        <v>8.5107890923543792</v>
+        <v>8.4758176674121</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1037,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="C59">
-        <v>8.1013348911375491</v>
+        <v>7.9431402271932301</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1048,7 +1048,7 @@
         <v>16</v>
       </c>
       <c r="C60">
-        <v>7.7715495705108104</v>
+        <v>7.7156543882285398</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1059,7 +1059,7 @@
         <v>20</v>
       </c>
       <c r="C61">
-        <v>7.5597380851924001</v>
+        <v>7.5391263421760897</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1070,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="C62">
-        <v>7.45562725101186</v>
+        <v>7.3295331842656601</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1081,7 +1081,7 @@
         <v>28</v>
       </c>
       <c r="C63">
-        <v>7.4138868138074603</v>
+        <v>7.46287237975229</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1092,7 +1092,7 @@
         <v>32</v>
       </c>
       <c r="C64">
-        <v>7.3988393882768504</v>
+        <v>7.5145104161657397</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1103,7 +1103,7 @@
         <v>36</v>
       </c>
       <c r="C65">
-        <v>7.39364520203904</v>
+        <v>7.5044683503598701</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1114,7 +1114,7 @@
         <v>40</v>
       </c>
       <c r="C66">
-        <v>7.3918802287706402</v>
+        <v>7.3524305746726002</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1125,7 +1125,7 @@
         <v>44</v>
       </c>
       <c r="C67">
-        <v>7.3912837501274202</v>
+        <v>7.3343135722739401</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1136,7 +1136,7 @@
         <v>48</v>
       </c>
       <c r="C68">
-        <v>7.3910825408566296</v>
+        <v>7.4347001858951201</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1147,7 +1147,7 @@
         <v>52</v>
       </c>
       <c r="C69">
-        <v>7.39101470970032</v>
+        <v>7.3359692926204199</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1158,7 +1158,7 @@
         <v>56</v>
       </c>
       <c r="C70">
-        <v>7.3909918474617404</v>
+        <v>7.42255225807848</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1169,7 +1169,7 @@
         <v>60</v>
       </c>
       <c r="C71">
-        <v>7.39098414237756</v>
+        <v>7.2711326582216396</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1180,7 +1180,7 @@
         <v>64</v>
       </c>
       <c r="C72">
-        <v>7.3909815456546504</v>
+        <v>7.5413405082406904</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>0.96160245846568204</v>
+        <v>1.23696799949033</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1202,7 +1202,7 @@
         <v>4</v>
       </c>
       <c r="C75">
-        <v>8.7648461134327107</v>
+        <v>8.7370768335883202</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1213,7 +1213,7 @@
         <v>8</v>
       </c>
       <c r="C76">
-        <v>8.3512646036982492</v>
+        <v>8.32648444044057</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1224,7 +1224,7 @@
         <v>12</v>
       </c>
       <c r="C77">
-        <v>7.9588736285508297</v>
+        <v>7.8705086554664403</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1235,7 +1235,7 @@
         <v>16</v>
       </c>
       <c r="C78">
-        <v>7.6132809136688504</v>
+        <v>7.6650396681457797</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1246,7 +1246,7 @@
         <v>20</v>
       </c>
       <c r="C79">
-        <v>7.3500168610102898</v>
+        <v>7.2873206597954301</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1257,7 +1257,7 @@
         <v>24</v>
       </c>
       <c r="C80">
-        <v>7.1879372963808699</v>
+        <v>7.1148441620736298</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1268,7 +1268,7 @@
         <v>28</v>
       </c>
       <c r="C81">
-        <v>7.1076074167913896</v>
+        <v>6.9468660799505999</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1279,7 +1279,7 @@
         <v>32</v>
       </c>
       <c r="C82">
-        <v>7.07341654713764</v>
+        <v>7.2037892012060798</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1290,7 +1290,7 @@
         <v>36</v>
       </c>
       <c r="C83">
-        <v>7.0599736262641102</v>
+        <v>6.9665962300496203</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1301,7 +1301,7 @@
         <v>40</v>
       </c>
       <c r="C84">
-        <v>7.0548668143266697</v>
+        <v>7.0858670456278903</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1312,7 +1312,7 @@
         <v>44</v>
       </c>
       <c r="C85">
-        <v>7.0529530016959603</v>
+        <v>7.1320873677772703</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1323,7 +1323,7 @@
         <v>48</v>
       </c>
       <c r="C86">
-        <v>7.0522394918548903</v>
+        <v>7.1633078271427699</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1334,7 +1334,7 @@
         <v>52</v>
       </c>
       <c r="C87">
-        <v>7.0519739966129604</v>
+        <v>7.1064179459534298</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1345,7 +1345,7 @@
         <v>56</v>
       </c>
       <c r="C88">
-        <v>7.0518752780649798</v>
+        <v>7.0281681453447202</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1356,7 +1356,7 @@
         <v>60</v>
       </c>
       <c r="C89">
-        <v>7.0518385816450904</v>
+        <v>7.1662868254810901</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>64</v>
       </c>
       <c r="C90">
-        <v>7.05182494193628</v>
+        <v>7.11975301287249</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>0.91102944323926205</v>
+        <v>0.87578462622748299</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1389,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="C93">
-        <v>6.8778156762135003</v>
+        <v>6.9067528085530698</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1400,7 +1400,7 @@
         <v>8</v>
       </c>
       <c r="C94">
-        <v>6.5463227763339704</v>
+        <v>6.7799489657851302</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1411,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="C95">
-        <v>6.3616865311564297</v>
+        <v>6.3736953835691796</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1422,7 +1422,7 @@
         <v>16</v>
       </c>
       <c r="C96">
-        <v>6.2927711110614801</v>
+        <v>6.3080607033614902</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1433,7 +1433,7 @@
         <v>20</v>
       </c>
       <c r="C97">
-        <v>6.2754036497338896</v>
+        <v>6.1324335387822604</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -1444,7 +1444,7 @@
         <v>24</v>
       </c>
       <c r="C98">
-        <v>6.2721022003897602</v>
+        <v>6.2694070715543999</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1455,7 +1455,7 @@
         <v>28</v>
       </c>
       <c r="C99">
-        <v>6.2715602855540498</v>
+        <v>6.3139928003686796</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -1466,7 +1466,7 @@
         <v>32</v>
       </c>
       <c r="C100">
-        <v>6.27147642878227</v>
+        <v>6.3696061632329499</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -1477,7 +1477,7 @@
         <v>36</v>
       </c>
       <c r="C101">
-        <v>6.2714637094573797</v>
+        <v>6.2956810795467701</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -1488,7 +1488,7 @@
         <v>40</v>
       </c>
       <c r="C102">
-        <v>6.2714617919735698</v>
+        <v>6.1927682539198603</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -1499,7 +1499,7 @@
         <v>44</v>
       </c>
       <c r="C103">
-        <v>6.271461503417</v>
+        <v>6.3083361755365601</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -1510,7 +1510,7 @@
         <v>48</v>
       </c>
       <c r="C104">
-        <v>6.2714614600144598</v>
+        <v>6.2627917514305098</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -1521,7 +1521,7 @@
         <v>52</v>
       </c>
       <c r="C105">
-        <v>6.2714614534870599</v>
+        <v>6.3637530284626802</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -1532,7 +1532,7 @@
         <v>56</v>
       </c>
       <c r="C106">
-        <v>6.27146145250543</v>
+        <v>6.3139522444202303</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -1543,7 +1543,7 @@
         <v>60</v>
       </c>
       <c r="C107">
-        <v>6.2714614523578103</v>
+        <v>6.3818272103545501</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -1554,7 +1554,7 @@
         <v>64</v>
       </c>
       <c r="C108">
-        <v>6.2714614523355996</v>
+        <v>6.1065049127241702</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <v>0.976542357660378</v>
+        <v>0.94059591059861103</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -1576,7 +1576,7 @@
         <v>4</v>
       </c>
       <c r="C111">
-        <v>7.9941561052043397</v>
+        <v>8.0285456317027997</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -1587,7 +1587,7 @@
         <v>8</v>
       </c>
       <c r="C112">
-        <v>7.6509949791896998</v>
+        <v>7.6867841463753903</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -1598,7 +1598,7 @@
         <v>12</v>
       </c>
       <c r="C113">
-        <v>7.3391811787763404</v>
+        <v>7.3543271126031904</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -1609,7 +1609,7 @@
         <v>16</v>
       </c>
       <c r="C114">
-        <v>7.0817238874543902</v>
+        <v>7.0030527916295</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -1620,7 +1620,7 @@
         <v>20</v>
       </c>
       <c r="C115">
-        <v>6.8982358814745099</v>
+        <v>6.5824033169443101</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -1631,7 +1631,7 @@
         <v>24</v>
       </c>
       <c r="C116">
-        <v>6.7885509685139196</v>
+        <v>6.7432519867470697</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -1642,7 +1642,7 @@
         <v>28</v>
       </c>
       <c r="C117">
-        <v>6.7325841516197702</v>
+        <v>6.6428388214135996</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -1653,7 +1653,7 @@
         <v>32</v>
       </c>
       <c r="C118">
-        <v>6.7069642434249701</v>
+        <v>6.6753265373064199</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -1664,7 +1664,7 @@
         <v>36</v>
       </c>
       <c r="C119">
-        <v>6.6959157922412</v>
+        <v>6.86898995934538</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -1675,7 +1675,7 @@
         <v>40</v>
       </c>
       <c r="C120">
-        <v>6.6912844806037404</v>
+        <v>6.87283470681054</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -1686,7 +1686,7 @@
         <v>44</v>
       </c>
       <c r="C121">
-        <v>6.6893671346058499</v>
+        <v>6.6444467404956802</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -1697,7 +1697,7 @@
         <v>48</v>
       </c>
       <c r="C122">
-        <v>6.6885775224140502</v>
+        <v>6.7851975330193897</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -1708,7 +1708,7 @@
         <v>52</v>
       </c>
       <c r="C123">
-        <v>6.6882530492611103</v>
+        <v>6.6212327332046899</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -1719,7 +1719,7 @@
         <v>56</v>
       </c>
       <c r="C124">
-        <v>6.68811983443344</v>
+        <v>6.4911788652670603</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -1730,7 +1730,7 @@
         <v>60</v>
       </c>
       <c r="C125">
-        <v>6.6880651623534302</v>
+        <v>6.8074401775819204</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -1741,7 +1741,7 @@
         <v>64</v>
       </c>
       <c r="C126">
-        <v>6.6880427280491004</v>
+        <v>6.6131914759357704</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="C128">
-        <v>0.94035535039481699</v>
+        <v>0.77492619277816999</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -1763,7 +1763,7 @@
         <v>4</v>
       </c>
       <c r="C129">
-        <v>8.9593506476776099</v>
+        <v>8.9062417308467996</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -1774,7 +1774,7 @@
         <v>8</v>
       </c>
       <c r="C130">
-        <v>8.7591674257770205</v>
+        <v>8.7112931809171599</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -1785,7 +1785,7 @@
         <v>12</v>
       </c>
       <c r="C131">
-        <v>8.5691960684113493</v>
+        <v>8.4435229776700105</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -1796,7 +1796,7 @@
         <v>16</v>
       </c>
       <c r="C132">
-        <v>8.3939661826109102</v>
+        <v>8.5480645964389605</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -1807,7 +1807,7 @@
         <v>20</v>
       </c>
       <c r="C133">
-        <v>8.2386060743979694</v>
+        <v>8.3878721099139995</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -1818,7 +1818,7 @@
         <v>24</v>
       </c>
       <c r="C134">
-        <v>8.1077023843557807</v>
+        <v>8.0969522282736008</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -1829,7 +1829,7 @@
         <v>28</v>
       </c>
       <c r="C135">
-        <v>8.0037610638211998</v>
+        <v>8.1265693567712205</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -1840,7 +1840,7 @@
         <v>32</v>
       </c>
       <c r="C136">
-        <v>7.9261711076462298</v>
+        <v>8.0146167342319199</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -1851,7 +1851,7 @@
         <v>36</v>
       </c>
       <c r="C137">
-        <v>7.8714685102990796</v>
+        <v>7.8033604514030301</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -1862,7 +1862,7 @@
         <v>40</v>
       </c>
       <c r="C138">
-        <v>7.8346863270130704</v>
+        <v>7.7832421426499696</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -1873,7 +1873,7 @@
         <v>44</v>
       </c>
       <c r="C139">
-        <v>7.8108231345068004</v>
+        <v>7.8733340043340698</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -1884,7 +1884,7 @@
         <v>48</v>
       </c>
       <c r="C140">
-        <v>7.7957256889771998</v>
+        <v>7.5482432007978302</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -1895,7 +1895,7 @@
         <v>52</v>
       </c>
       <c r="C141">
-        <v>7.7863327773570603</v>
+        <v>7.6888943136291097</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -1906,7 +1906,7 @@
         <v>56</v>
       </c>
       <c r="C142">
-        <v>7.7805516272050603</v>
+        <v>7.6385971498196001</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -1917,7 +1917,7 @@
         <v>60</v>
       </c>
       <c r="C143">
-        <v>7.7770174786113904</v>
+        <v>7.7771010815331101</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
@@ -1928,7 +1928,7 @@
         <v>64</v>
       </c>
       <c r="C144">
-        <v>7.7748660234713798</v>
+        <v>7.9028610483590498</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="C146">
-        <v>1.0853679417846001</v>
+        <v>1.2710394732004799</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -1950,7 +1950,7 @@
         <v>4</v>
       </c>
       <c r="C147">
-        <v>7.9030535474498604</v>
+        <v>7.8274966013857004</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
@@ -1961,7 +1961,7 @@
         <v>8</v>
       </c>
       <c r="C148">
-        <v>7.5853707040704599</v>
+        <v>7.6468522685102904</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -1972,7 +1972,7 @@
         <v>12</v>
       </c>
       <c r="C149">
-        <v>7.3563124144033099</v>
+        <v>7.3084868992777299</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -1983,7 +1983,7 @@
         <v>16</v>
       </c>
       <c r="C150">
-        <v>7.2233495761715396</v>
+        <v>7.1130709429736099</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -1994,7 +1994,7 @@
         <v>20</v>
       </c>
       <c r="C151">
-        <v>7.1601473874001096</v>
+        <v>7.1184000724943903</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -2005,7 +2005,7 @@
         <v>24</v>
       </c>
       <c r="C152">
-        <v>7.1337729439013096</v>
+        <v>7.1556132253207698</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -2016,7 +2016,7 @@
         <v>28</v>
       </c>
       <c r="C153">
-        <v>7.1234596823279803</v>
+        <v>7.1188183748055103</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -2027,7 +2027,7 @@
         <v>32</v>
       </c>
       <c r="C154">
-        <v>7.1195369601606897</v>
+        <v>7.1520236417869896</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -2038,7 +2038,7 @@
         <v>36</v>
       </c>
       <c r="C155">
-        <v>7.1180611116427901</v>
+        <v>7.1069443317709098</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -2049,7 +2049,7 @@
         <v>40</v>
       </c>
       <c r="C156">
-        <v>7.1175081576678201</v>
+        <v>7.07609834259764</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -2060,7 +2060,7 @@
         <v>44</v>
       </c>
       <c r="C157">
-        <v>7.1173013078654899</v>
+        <v>7.1579677590156896</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
@@ -2071,7 +2071,7 @@
         <v>48</v>
       </c>
       <c r="C158">
-        <v>7.1172239746462402</v>
+        <v>7.0563114774705999</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -2082,7 +2082,7 @@
         <v>52</v>
       </c>
       <c r="C159">
-        <v>7.1171950690712604</v>
+        <v>7.2006792608593102</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -2093,7 +2093,7 @@
         <v>56</v>
       </c>
       <c r="C160">
-        <v>7.11718426564663</v>
+        <v>6.8909852465833596</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -2104,7 +2104,7 @@
         <v>60</v>
       </c>
       <c r="C161">
-        <v>7.1171802280034102</v>
+        <v>7.1701008392569801</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -2115,7 +2115,7 @@
         <v>64</v>
       </c>
       <c r="C162">
-        <v>7.1171787190026903</v>
+        <v>7.1171645896990103</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="C164">
-        <v>0.81920268111331296</v>
+        <v>0.77066560594210798</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
@@ -2137,7 +2137,7 @@
         <v>4</v>
       </c>
       <c r="C165">
-        <v>8.3196202660818095</v>
+        <v>8.1953751639928107</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -2148,7 +2148,7 @@
         <v>8</v>
       </c>
       <c r="C166">
-        <v>8.0358362899951405</v>
+        <v>8.0763946656543002</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -2159,7 +2159,7 @@
         <v>12</v>
       </c>
       <c r="C167">
-        <v>7.8146806653514496</v>
+        <v>7.87188273462022</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -2170,7 +2170,7 @@
         <v>16</v>
       </c>
       <c r="C168">
-        <v>7.6675830132764702</v>
+        <v>7.7360860239387099</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -2181,7 +2181,7 @@
         <v>20</v>
       </c>
       <c r="C169">
-        <v>7.5844020649334603</v>
+        <v>7.6172974169406196</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -2192,7 +2192,7 @@
         <v>24</v>
       </c>
       <c r="C170">
-        <v>7.5428844317266002</v>
+        <v>7.8594599758059598</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
@@ -2203,7 +2203,7 @@
         <v>28</v>
       </c>
       <c r="C171">
-        <v>7.52366995288138</v>
+        <v>7.6677370767198898</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
@@ -2214,7 +2214,7 @@
         <v>32</v>
       </c>
       <c r="C172">
-        <v>7.5151163294305503</v>
+        <v>7.4785279186680702</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
@@ -2225,7 +2225,7 @@
         <v>36</v>
       </c>
       <c r="C173">
-        <v>7.5113772814973903</v>
+        <v>7.52476760721785</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
@@ -2236,7 +2236,7 @@
         <v>40</v>
       </c>
       <c r="C174">
-        <v>7.50975610310637</v>
+        <v>7.6160698448014497</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
@@ -2247,7 +2247,7 @@
         <v>44</v>
       </c>
       <c r="C175">
-        <v>7.5090556984684502</v>
+        <v>7.5332067473373003</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
@@ -2258,7 +2258,7 @@
         <v>48</v>
       </c>
       <c r="C176">
-        <v>7.5087535685017102</v>
+        <v>7.44379104520391</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
@@ -2269,7 +2269,7 @@
         <v>52</v>
       </c>
       <c r="C177">
-        <v>7.5086233275865197</v>
+        <v>7.5472959168733</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
@@ -2280,7 +2280,7 @@
         <v>56</v>
       </c>
       <c r="C178">
-        <v>7.5085672039942599</v>
+        <v>7.5921097434623901</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
@@ -2291,7 +2291,7 @@
         <v>60</v>
       </c>
       <c r="C179">
-        <v>7.5085430237919297</v>
+        <v>7.5600961600727299</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
@@ -2302,7 +2302,7 @@
         <v>64</v>
       </c>
       <c r="C180">
-        <v>7.5085326021907504</v>
+        <v>7.5925235984262303</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="C182">
-        <v>1.2866125494448799</v>
+        <v>1.1504864887598001</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
@@ -2324,7 +2324,7 @@
         <v>4</v>
       </c>
       <c r="C183">
-        <v>8.7123759764828801</v>
+        <v>8.6374932958304207</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
@@ -2335,7 +2335,7 @@
         <v>8</v>
       </c>
       <c r="C184">
-        <v>8.3834806800341202</v>
+        <v>8.2464785858850007</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
@@ -2346,7 +2346,7 @@
         <v>12</v>
       </c>
       <c r="C185">
-        <v>8.0739311968416594</v>
+        <v>8.2664643335757795</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
@@ -2357,7 +2357,7 @@
         <v>16</v>
       </c>
       <c r="C186">
-        <v>7.7997338492093702</v>
+        <v>7.7034434365108702</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
@@ -2368,7 +2368,7 @@
         <v>20</v>
       </c>
       <c r="C187">
-        <v>7.5802913244064598</v>
+        <v>7.4522484389993</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
@@ -2379,7 +2379,7 @@
         <v>24</v>
       </c>
       <c r="C188">
-        <v>7.4277780944206002</v>
+        <v>7.3731661104580999</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
@@ -2390,7 +2390,7 @@
         <v>28</v>
       </c>
       <c r="C189">
-        <v>7.3371006727646702</v>
+        <v>7.2612776883476799</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
@@ -2401,7 +2401,7 @@
         <v>32</v>
       </c>
       <c r="C190">
-        <v>7.28999790149952</v>
+        <v>7.35614566652644</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
@@ -2412,7 +2412,7 @@
         <v>36</v>
       </c>
       <c r="C191">
-        <v>7.2676896443814396</v>
+        <v>7.0803077829783598</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
@@ -2423,7 +2423,7 @@
         <v>40</v>
       </c>
       <c r="C192">
-        <v>7.2576615608663699</v>
+        <v>7.2590791266396204</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
@@ -2434,7 +2434,7 @@
         <v>44</v>
       </c>
       <c r="C193">
-        <v>7.2532687894615702</v>
+        <v>7.3498001683183398</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -2445,7 +2445,7 @@
         <v>48</v>
       </c>
       <c r="C194">
-        <v>7.25136728559748</v>
+        <v>7.26269845315952</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
@@ -2456,7 +2456,7 @@
         <v>52</v>
       </c>
       <c r="C195">
-        <v>7.2505484974444796</v>
+        <v>7.3634832629052198</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -2467,7 +2467,7 @@
         <v>56</v>
       </c>
       <c r="C196">
-        <v>7.2501967326418697</v>
+        <v>7.2693224396131102</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
@@ -2478,7 +2478,7 @@
         <v>60</v>
       </c>
       <c r="C197">
-        <v>7.25004575780153</v>
+        <v>7.2986556687496904</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
@@ -2489,7 +2489,7 @@
         <v>64</v>
       </c>
       <c r="C198">
-        <v>7.2499809880094102</v>
+        <v>7.2696818662659597</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
@@ -2500,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="C200">
-        <v>1.03557290213743</v>
+        <v>0.97679589946663403</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
@@ -2511,7 +2511,7 @@
         <v>4</v>
       </c>
       <c r="C201">
-        <v>8.7144823441947601</v>
+        <v>8.7765089309838604</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
@@ -2522,7 +2522,7 @@
         <v>8</v>
       </c>
       <c r="C202">
-        <v>8.4642487360177103</v>
+        <v>8.4678587326910097</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
@@ -2533,7 +2533,7 @@
         <v>12</v>
       </c>
       <c r="C203">
-        <v>8.2191937130986705</v>
+        <v>8.0238333856253004</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
@@ -2544,7 +2544,7 @@
         <v>16</v>
       </c>
       <c r="C204">
-        <v>7.9829417812886501</v>
+        <v>7.9443689361281002</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -2555,7 +2555,7 @@
         <v>20</v>
       </c>
       <c r="C205">
-        <v>7.7610162316350202</v>
+        <v>7.7836583733545499</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -2566,7 +2566,7 @@
         <v>24</v>
       </c>
       <c r="C206">
-        <v>7.5608593741980501</v>
+        <v>7.48540038155065</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
@@ -2577,7 +2577,7 @@
         <v>28</v>
       </c>
       <c r="C207">
-        <v>7.3906268782541202</v>
+        <v>7.3860523605602904</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -2588,7 +2588,7 @@
         <v>32</v>
       </c>
       <c r="C208">
-        <v>7.2564263584207804</v>
+        <v>7.2494508769590498</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
@@ -2599,7 +2599,7 @@
         <v>36</v>
       </c>
       <c r="C209">
-        <v>7.1593457253638402</v>
+        <v>7.3187998700502597</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
@@ -2610,7 +2610,7 @@
         <v>40</v>
       </c>
       <c r="C210">
-        <v>7.0947880483039496</v>
+        <v>7.2943416698976797</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -2621,7 +2621,7 @@
         <v>44</v>
       </c>
       <c r="C211">
-        <v>7.0548111559534297</v>
+        <v>6.9762231254136298</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
@@ -2632,7 +2632,7 @@
         <v>48</v>
       </c>
       <c r="C212">
-        <v>7.0313301100103001</v>
+        <v>7.06146213166745</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -2643,7 +2643,7 @@
         <v>52</v>
       </c>
       <c r="C213">
-        <v>7.0180146228258202</v>
+        <v>6.9553332879177603</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
@@ -2654,7 +2654,7 @@
         <v>56</v>
       </c>
       <c r="C214">
-        <v>7.0106250550008404</v>
+        <v>7.0703716956116303</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -2665,7 +2665,7 @@
         <v>60</v>
       </c>
       <c r="C215">
-        <v>7.0065753776824202</v>
+        <v>7.1256983096734698</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
@@ -2676,7 +2676,7 @@
         <v>64</v>
       </c>
       <c r="C216">
-        <v>7.0043717151816498</v>
+        <v>7.1899627281037297</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="C218">
-        <v>1.20793966910719</v>
+        <v>1.2503920843533201</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -2698,7 +2698,7 @@
         <v>4</v>
       </c>
       <c r="C219">
-        <v>7.6920757611560404</v>
+        <v>7.5458574483448801</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
@@ -2709,7 +2709,7 @@
         <v>8</v>
       </c>
       <c r="C220">
-        <v>7.30046272001504</v>
+        <v>7.2672744118402797</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
@@ -2720,7 +2720,7 @@
         <v>12</v>
       </c>
       <c r="C221">
-        <v>6.93676863882036</v>
+        <v>7.0606449386537697</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
@@ -2731,7 +2731,7 @@
         <v>16</v>
       </c>
       <c r="C222">
-        <v>6.6249363016254996</v>
+        <v>6.7354344475253196</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
@@ -2742,7 +2742,7 @@
         <v>20</v>
       </c>
       <c r="C223">
-        <v>6.3909412821320704</v>
+        <v>6.4616262542851697</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
@@ -2753,7 +2753,7 @@
         <v>24</v>
       </c>
       <c r="C224">
-        <v>6.2484964924789201</v>
+        <v>6.3489989618411</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
@@ -2764,7 +2764,7 @@
         <v>28</v>
       </c>
       <c r="C225">
-        <v>6.1883471500876803</v>
+        <v>6.2591960412796697</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
@@ -2775,7 +2775,7 @@
         <v>32</v>
       </c>
       <c r="C226">
-        <v>6.1810097466226797</v>
+        <v>6.0685635752414502</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
@@ -2786,7 +2786,7 @@
         <v>36</v>
       </c>
       <c r="C227">
-        <v>6.19284401457546</v>
+        <v>6.3170013080594396</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -2797,7 +2797,7 @@
         <v>40</v>
       </c>
       <c r="C228">
-        <v>6.20297111796528</v>
+        <v>6.0574639964033299</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
@@ -2808,7 +2808,7 @@
         <v>44</v>
       </c>
       <c r="C229">
-        <v>6.20640508354019</v>
+        <v>6.30154811780399</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
@@ -2819,7 +2819,7 @@
         <v>48</v>
       </c>
       <c r="C230">
-        <v>6.2059000774208499</v>
+        <v>6.2050280261505799</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -2830,7 +2830,7 @@
         <v>52</v>
       </c>
       <c r="C231">
-        <v>6.2046265493581396</v>
+        <v>6.2248895847870198</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -2841,7 +2841,7 @@
         <v>56</v>
       </c>
       <c r="C232">
-        <v>6.2039153917430099</v>
+        <v>6.0969702725847696</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -2852,7 +2852,7 @@
         <v>60</v>
       </c>
       <c r="C233">
-        <v>6.2037895337665097</v>
+        <v>6.3121577751003999</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -2863,7 +2863,7 @@
         <v>64</v>
       </c>
       <c r="C234">
-        <v>6.2039005883747302</v>
+        <v>6.0627928704857101</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
       <c r="C236">
-        <v>1.0076051919381701</v>
+        <v>0.90348828174979201</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
@@ -2885,7 +2885,7 @@
         <v>4</v>
       </c>
       <c r="C237">
-        <v>7.9474550419516303</v>
+        <v>8.05109086682784</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -2896,7 +2896,7 @@
         <v>8</v>
       </c>
       <c r="C238">
-        <v>7.4376193175748302</v>
+        <v>7.4765408964823399</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
@@ -2907,7 +2907,7 @@
         <v>12</v>
       </c>
       <c r="C239">
-        <v>7.1039794382579498</v>
+        <v>7.1392731025672003</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
@@ -2918,7 +2918,7 @@
         <v>16</v>
       </c>
       <c r="C240">
-        <v>6.9635708371905398</v>
+        <v>7.0886682779723804</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
@@ -2929,7 +2929,7 @@
         <v>20</v>
       </c>
       <c r="C241">
-        <v>6.9226443524091303</v>
+        <v>6.9266160127947503</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
@@ -2940,7 +2940,7 @@
         <v>24</v>
       </c>
       <c r="C242">
-        <v>6.91253204651749</v>
+        <v>6.9090332559869498</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
@@ -2951,7 +2951,7 @@
         <v>28</v>
       </c>
       <c r="C243">
-        <v>6.9101529085193496</v>
+        <v>6.8610239058046902</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
@@ -2962,7 +2962,7 @@
         <v>32</v>
       </c>
       <c r="C244">
-        <v>6.9095999291465997</v>
+        <v>6.8624093253265599</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
@@ -2973,7 +2973,7 @@
         <v>36</v>
       </c>
       <c r="C245">
-        <v>6.9094717685148002</v>
+        <v>7.0073790655326498</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
@@ -2984,7 +2984,7 @@
         <v>40</v>
       </c>
       <c r="C246">
-        <v>6.9094420852798297</v>
+        <v>6.9769660297127096</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
@@ -2995,7 +2995,7 @@
         <v>44</v>
       </c>
       <c r="C247">
-        <v>6.9094352114178301</v>
+        <v>6.8466481612303198</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
@@ -3006,7 +3006,7 @@
         <v>48</v>
       </c>
       <c r="C248">
-        <v>6.9094336196677899</v>
+        <v>6.8894556659292903</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
@@ -3017,7 +3017,7 @@
         <v>52</v>
       </c>
       <c r="C249">
-        <v>6.9094332510762797</v>
+        <v>6.7968186899271599</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
@@ -3028,7 +3028,7 @@
         <v>56</v>
       </c>
       <c r="C250">
-        <v>6.90943316572403</v>
+        <v>6.7060557698801002</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
@@ -3039,7 +3039,7 @@
         <v>60</v>
       </c>
       <c r="C251">
-        <v>6.9094331459595999</v>
+        <v>6.8634234606835802</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
@@ -3050,7 +3050,7 @@
         <v>64</v>
       </c>
       <c r="C252">
-        <v>6.9094331413828796</v>
+        <v>6.8503363233767498</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
@@ -3061,7 +3061,7 @@
         <v>0</v>
       </c>
       <c r="C254">
-        <v>0.81852984947638396</v>
+        <v>0.84405174654729997</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -3072,7 +3072,7 @@
         <v>4</v>
       </c>
       <c r="C255">
-        <v>7.8009399506444099</v>
+        <v>7.6485307315252102</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
@@ -3083,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="C256">
-        <v>7.4010702344516597</v>
+        <v>7.6110398129145498</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
@@ -3094,7 +3094,7 @@
         <v>12</v>
       </c>
       <c r="C257">
-        <v>7.0703672584917099</v>
+        <v>7.0331127010464698</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
@@ -3105,7 +3105,7 @@
         <v>16</v>
       </c>
       <c r="C258">
-        <v>6.8462428736110104</v>
+        <v>6.6768043052682797</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
@@ -3116,7 +3116,7 @@
         <v>20</v>
       </c>
       <c r="C259">
-        <v>6.7294820807747104</v>
+        <v>6.7176946177769397</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
@@ -3127,7 +3127,7 @@
         <v>24</v>
       </c>
       <c r="C260">
-        <v>6.6818646560984396</v>
+        <v>6.7096544311091</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
@@ -3138,7 +3138,7 @@
         <v>28</v>
       </c>
       <c r="C261">
-        <v>6.6652896747180401</v>
+        <v>6.7919785627822904</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
@@ -3149,7 +3149,7 @@
         <v>32</v>
       </c>
       <c r="C262">
-        <v>6.6599312192400504</v>
+        <v>6.9710852484438002</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
@@ -3160,7 +3160,7 @@
         <v>36</v>
       </c>
       <c r="C263">
-        <v>6.6582459546566897</v>
+        <v>6.7022002249874397</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
@@ -3171,7 +3171,7 @@
         <v>40</v>
       </c>
       <c r="C264">
-        <v>6.6577207553187199</v>
+        <v>6.5765148478834003</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
@@ -3182,7 +3182,7 @@
         <v>44</v>
       </c>
       <c r="C265">
-        <v>6.6575575557022404</v>
+        <v>6.7036600490162401</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
@@ -3193,7 +3193,7 @@
         <v>48</v>
       </c>
       <c r="C266">
-        <v>6.6575068893203104</v>
+        <v>6.5345399175811698</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
@@ -3204,7 +3204,7 @@
         <v>52</v>
       </c>
       <c r="C267">
-        <v>6.6574911640528702</v>
+        <v>6.6177935594694501</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
@@ -3215,7 +3215,7 @@
         <v>56</v>
       </c>
       <c r="C268">
-        <v>6.6574862838473496</v>
+        <v>6.6703770475214998</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
@@ -3226,7 +3226,7 @@
         <v>60</v>
       </c>
       <c r="C269">
-        <v>6.6574847693575201</v>
+        <v>6.8150492791138104</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
@@ -3237,7 +3237,7 @@
         <v>64</v>
       </c>
       <c r="C270">
-        <v>6.6574842993649899</v>
+        <v>6.5761510033466797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>